<commit_message>
Fixed two-way analysis and added global test on means
</commit_message>
<xml_diff>
--- a/problem_1/Problem 1 to delivery-20240322/balanced_sample.xlsx
+++ b/problem_1/Problem 1 to delivery-20240322/balanced_sample.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matulda/Desktop/FCUL/Semester 2/Regression and Analysis of Variance /HA 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D48825E-EE3D-6942-A901-463BBB96187D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C900AF3B-5018-EE4C-94BC-72D6CDC2916D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="17540" windowHeight="17220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Two way analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="Global test on means" sheetId="4" r:id="rId2"/>
+    <sheet name="Two way analysis" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +34,57 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0B0AB79D-7A38-2F4C-B1C6-C9726E753C50}</author>
+    <author>tc={A90F0769-4B2A-5943-9D26-887AE9D180D1}</author>
+  </authors>
+  <commentList>
+    <comment ref="N19" authorId="0" shapeId="0" xr:uid="{0B0AB79D-7A38-2F4C-B1C6-C9726E753C50}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    There are differences between means.</t>
+      </text>
+    </comment>
+    <comment ref="N30" authorId="1" shapeId="0" xr:uid="{A90F0769-4B2A-5943-9D26-887AE9D180D1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    There are differences between means.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BA6F67CF-88E3-5848-9BC8-6985B487C04E}</author>
+  </authors>
+  <commentList>
+    <comment ref="G32" authorId="0" shapeId="0" xr:uid="{BA6F67CF-88E3-5848-9BC8-6985B487C04E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not correct??? 
+Reply:
+    So apparently, when they are not equal, it suggests no interaction between the factors, which is also “proved” in H03 - we cannot reject, and on the graphs we do not see clear interaction (besides mby typical and fair? But lets say not haha) 
+Reply:
+    Okay never mind, it has nothing to do with the interaction, chatGPT lied to me, I just made a mistake</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="64">
   <si>
     <t>SalePrice</t>
   </si>
@@ -148,13 +198,94 @@
   </si>
   <si>
     <t>SS_FactA+SS_FactB+SSInt</t>
+  </si>
+  <si>
+    <t>H01: The a effects of A are all null.</t>
+  </si>
+  <si>
+    <t>H0</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>H02: The b effects of B are all null</t>
+  </si>
+  <si>
+    <t>H03: No interaction between factor A and factor B</t>
+  </si>
+  <si>
+    <t>Fair</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Typical</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Significance level</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>model 1</t>
+  </si>
+  <si>
+    <t>model 2</t>
+  </si>
+  <si>
+    <t>Alphas:</t>
+  </si>
+  <si>
+    <t>Are there differences between the means of the groups?</t>
+  </si>
+  <si>
+    <t>Sum of Alphas</t>
+  </si>
+  <si>
+    <t>miu^</t>
+  </si>
+  <si>
+    <t>sigma2</t>
+  </si>
+  <si>
+    <t>F-ratio</t>
+  </si>
+  <si>
+    <t>Treat</t>
+  </si>
+  <si>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>H0: miu1=miu2=…=miu6</t>
+  </si>
+  <si>
+    <t>H0: alpha1=alpha2=…=alpha6=0</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,6 +335,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -237,7 +390,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -547,26 +700,84 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="double">
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -578,7 +789,29 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -590,108 +823,138 @@
       <right style="double">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="1">
-      <left style="thin">
+      <left style="double">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal style="thin">
         <color indexed="64"/>
       </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -715,12 +978,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -731,31 +988,281 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{82080F7A-3033-9C4D-92F9-BCA666EF0E82}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -810,7 +1317,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Chart Title</a:t>
+              <a:t>Sale price based on presence of central airconditioning</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -886,13 +1393,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Fa</c:v>
+                  <c:v>Fair</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Gd</c:v>
+                  <c:v>Good</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TA</c:v>
+                  <c:v>Typical</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -958,13 +1465,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Fa</c:v>
+                  <c:v>Fair</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Gd</c:v>
+                  <c:v>Good</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TA</c:v>
+                  <c:v>Typical</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1212,6 +1719,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Sale</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> price based on kitchen quality</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1256,7 +1792,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fa</c:v>
+                  <c:v>Fair</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1291,10 +1827,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>N</c:v>
+                  <c:v>No</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Y</c:v>
+                  <c:v>Yes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1330,7 +1866,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gd</c:v>
+                  <c:v>Good</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1365,10 +1901,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>N</c:v>
+                  <c:v>No</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Y</c:v>
+                  <c:v>Yes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1404,7 +1940,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TA</c:v>
+                  <c:v>Typical</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1439,10 +1975,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>N</c:v>
+                  <c:v>No</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Y</c:v>
+                  <c:v>Yes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2837,6 +3373,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="fc62607" id="{80439527-ED8F-1B48-B4F5-C54134A98A16}" userId="S::fc62607@alunos.fc.ul.pt::0e3e20e6-f693-4309-97ed-422933c7062f" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3114,12 +3656,38 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="N19" dT="2024-04-01T03:11:38.04" personId="{80439527-ED8F-1B48-B4F5-C54134A98A16}" id="{0B0AB79D-7A38-2F4C-B1C6-C9726E753C50}">
+    <text>There are differences between means.</text>
+  </threadedComment>
+  <threadedComment ref="N30" dT="2024-04-01T03:11:33.30" personId="{80439527-ED8F-1B48-B4F5-C54134A98A16}" id="{A90F0769-4B2A-5943-9D26-887AE9D180D1}">
+    <text>There are differences between means.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G32" dT="2024-03-31T18:35:52.00" personId="{80439527-ED8F-1B48-B4F5-C54134A98A16}" id="{BA6F67CF-88E3-5848-9BC8-6985B487C04E}">
+    <text xml:space="preserve">Not correct??? 
+</text>
+  </threadedComment>
+  <threadedComment ref="G32" dT="2024-04-01T02:05:59.26" personId="{80439527-ED8F-1B48-B4F5-C54134A98A16}" id="{BBB784B1-2FF4-B441-8D23-21C7E1EF0AC3}" parentId="{BA6F67CF-88E3-5848-9BC8-6985B487C04E}">
+    <text xml:space="preserve">So apparently, when they are not equal, it suggests no interaction between the factors, which is also “proved” in H03 - we cannot reject, and on the graphs we do not see clear interaction (besides mby typical and fair? But lets say not haha) </text>
+  </threadedComment>
+  <threadedComment ref="G32" dT="2024-04-01T03:56:27.32" personId="{80439527-ED8F-1B48-B4F5-C54134A98A16}" id="{A1D95325-E9F0-8147-B8D6-4B8D1909E1F4}" parentId="{BA6F67CF-88E3-5848-9BC8-6985B487C04E}">
+    <text>Okay never mind, it has nothing to do with the interaction, chatGPT lied to me, I just made a mistake</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I20"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3134,11 +3702,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="22"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -3150,11 +3718,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3168,16 +3736,16 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="45" t="s">
         <v>4</v>
       </c>
       <c r="H3">
         <v>5.25</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="7">
         <v>11.75</v>
       </c>
     </row>
@@ -3191,22 +3759,22 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="46"/>
       <c r="H4">
         <v>12.1</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="7">
         <v>14.99</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
     </row>
     <row r="5" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3218,22 +3786,22 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="8"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="46"/>
       <c r="H5">
         <v>8.1999999999999993</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="7">
         <v>7.65</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="4" t="s">
+      <c r="P5" s="49"/>
+      <c r="Q5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3247,27 +3815,27 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="8"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="46"/>
       <c r="H6">
         <v>5.5993000000000004</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="7">
         <v>13.75</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="P6" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="2">
         <v>130</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="2">
         <v>150</v>
       </c>
-      <c r="S6" s="7">
+      <c r="S6" s="2">
         <v>138</v>
       </c>
     </row>
@@ -3281,23 +3849,23 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="46"/>
       <c r="H7">
         <v>8.5</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="7">
         <v>20</v>
       </c>
-      <c r="O7" s="5"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="7">
+      <c r="O7" s="51"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="2">
         <v>155</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="2">
         <v>188</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S7" s="2">
         <v>110</v>
       </c>
     </row>
@@ -3311,23 +3879,23 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="17">
+      <c r="F8" s="42"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="6">
         <v>14</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="8">
         <v>11.6</v>
       </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="7">
+      <c r="O8" s="51"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="2">
         <v>74</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="2">
         <v>159</v>
       </c>
-      <c r="S8" s="7">
+      <c r="S8" s="2">
         <v>168</v>
       </c>
     </row>
@@ -3341,25 +3909,25 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="42"/>
+      <c r="G9" s="46" t="s">
         <v>5</v>
       </c>
       <c r="H9">
         <v>21.45</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="7">
         <v>14.7</v>
       </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10">
+      <c r="O9" s="51"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="3">
         <v>180</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="3">
         <v>126</v>
       </c>
-      <c r="S9" s="10">
+      <c r="S9" s="3">
         <v>160</v>
       </c>
     </row>
@@ -3373,25 +3941,25 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="46"/>
       <c r="H10">
         <v>16.75</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="7">
         <v>22</v>
       </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="11" t="s">
+      <c r="O10" s="51"/>
+      <c r="P10" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="2">
         <v>34</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="2">
         <v>136</v>
       </c>
-      <c r="S10" s="7">
+      <c r="S10" s="2">
         <v>174</v>
       </c>
     </row>
@@ -3405,23 +3973,23 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="46"/>
       <c r="H11">
         <v>20.5</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="7">
         <v>28.7</v>
       </c>
-      <c r="O11" s="5"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="7">
+      <c r="O11" s="51"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="2">
         <v>40</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="2">
         <v>122</v>
       </c>
-      <c r="S11" s="7">
+      <c r="S11" s="2">
         <v>120</v>
       </c>
     </row>
@@ -3435,23 +4003,23 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="46"/>
       <c r="H12">
         <v>26.597899999999999</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="7">
         <v>24.4</v>
       </c>
-      <c r="O12" s="5"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="7">
+      <c r="O12" s="51"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="2">
         <v>80</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="2">
         <v>106</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="2">
         <v>150</v>
       </c>
     </row>
@@ -3465,23 +4033,23 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="46"/>
       <c r="H13">
         <v>21.45</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="7">
         <v>23.9</v>
       </c>
-      <c r="O13" s="5"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="10">
+      <c r="O13" s="51"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="3">
         <v>75</v>
       </c>
-      <c r="R13" s="10">
+      <c r="R13" s="3">
         <v>115</v>
       </c>
-      <c r="S13" s="10">
+      <c r="S13" s="3">
         <v>139</v>
       </c>
     </row>
@@ -3495,25 +4063,25 @@
       <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="17">
+      <c r="F14" s="42"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="6">
         <v>21.45</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="8">
         <v>43.715400000000002</v>
       </c>
-      <c r="O14" s="5"/>
-      <c r="P14" s="11" t="s">
+      <c r="O14" s="51"/>
+      <c r="P14" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="Q14" s="2">
         <v>20</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R14" s="2">
         <v>25</v>
       </c>
-      <c r="S14" s="7">
+      <c r="S14" s="2">
         <v>96</v>
       </c>
     </row>
@@ -3527,25 +4095,25 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="8" t="s">
+      <c r="F15" s="42"/>
+      <c r="G15" s="46" t="s">
         <v>6</v>
       </c>
       <c r="H15">
         <v>12.6</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="7">
         <v>12.3</v>
       </c>
-      <c r="O15" s="5"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="7">
+      <c r="O15" s="51"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="2">
         <v>70</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="2">
         <v>70</v>
       </c>
-      <c r="S15" s="7">
+      <c r="S15" s="2">
         <v>104</v>
       </c>
     </row>
@@ -3559,23 +4127,23 @@
       <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="46"/>
       <c r="H16">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="7">
         <v>18.05</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="7">
+      <c r="O16" s="51"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="2">
         <v>82</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R16" s="2">
         <v>58</v>
       </c>
-      <c r="S16" s="7">
+      <c r="S16" s="2">
         <v>82</v>
       </c>
     </row>
@@ -3589,23 +4157,23 @@
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="8"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="46"/>
       <c r="H17">
         <v>10.6</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="7">
         <v>10.95</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="10">
+      <c r="O17" s="51"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="3">
         <v>58</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="3">
         <v>45</v>
       </c>
-      <c r="S17" s="10">
+      <c r="S17" s="3">
         <v>60</v>
       </c>
     </row>
@@ -3619,12 +4187,12 @@
       <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="46"/>
       <c r="H18">
         <v>4</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="7">
         <v>19</v>
       </c>
     </row>
@@ -3638,12 +4206,12 @@
       <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="8"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="46"/>
       <c r="H19">
         <v>8.6999999999999993</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="7">
         <v>12.8</v>
       </c>
     </row>
@@ -3657,12 +4225,12 @@
       <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="17">
+      <c r="F20" s="42"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="6">
         <v>10.199999999999999</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="8">
         <v>11.92</v>
       </c>
     </row>
@@ -3676,7 +4244,6 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -3856,17 +4423,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F3:F20"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="G9:G14"/>
-    <mergeCell ref="G15:G20"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="O6:O17"/>
     <mergeCell ref="P6:P9"/>
     <mergeCell ref="P10:P13"/>
     <mergeCell ref="P14:P17"/>
+    <mergeCell ref="F3:F20"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="G9:G14"/>
+    <mergeCell ref="G15:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3874,596 +4441,1326 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F43188-026E-7742-AA92-2FD306518DEB}">
-  <dimension ref="A1:O27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FDD8E0-6B49-6E4B-87CB-FB3DC7D9BEEB}">
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="G1" s="29" t="s">
+      <c r="D1" s="44"/>
+      <c r="G1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="30">
+      <c r="F2" s="7"/>
+      <c r="G2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="11">
         <f>AVERAGE(C3:C8)</f>
         <v>8.9415499999999994</v>
       </c>
-      <c r="I2" s="30">
+      <c r="I2" s="11">
         <f>AVERAGE(D3:D8)</f>
         <v>13.29</v>
       </c>
-      <c r="J2" s="31">
+    </row>
+    <row r="3" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5.25</v>
+      </c>
+      <c r="D3" s="7">
+        <v>11.75</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="15">
+        <f>AVERAGE(C9:C14)</f>
+        <v>21.366316666666666</v>
+      </c>
+      <c r="I3" s="15">
+        <f>AVERAGE(D9:D14)</f>
+        <v>26.235900000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="59"/>
+      <c r="B4" s="46"/>
+      <c r="C4">
+        <v>12.1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>14.99</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="17">
+        <f>AVERAGE(C15:C20)</f>
+        <v>9.3166666666666682</v>
+      </c>
+      <c r="I4" s="17">
+        <f>AVERAGE(D15:D20)</f>
+        <v>14.17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="59"/>
+      <c r="B5" s="46"/>
+      <c r="C5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D5" s="7">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="59"/>
+      <c r="B6" s="46"/>
+      <c r="C6">
+        <v>5.5993000000000004</v>
+      </c>
+      <c r="D6" s="7">
+        <v>13.75</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="59"/>
+      <c r="B7" s="46"/>
+      <c r="C7">
+        <v>8.5</v>
+      </c>
+      <c r="D7" s="7">
+        <v>20</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="34"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="59"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="6">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8">
+        <v>11.6</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="30">
+        <f>DEVSQ(C3:C8)</f>
+        <v>61.106762074999999</v>
+      </c>
+      <c r="I8" s="31">
+        <f>DEVSQ(D3:D8)</f>
+        <v>85.163000000000011</v>
+      </c>
+      <c r="J8" s="35"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="59"/>
+      <c r="B9" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>21.45</v>
+      </c>
+      <c r="D9" s="7">
+        <v>14.7</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="32">
+        <f>DEVSQ(C9:C14)</f>
+        <v>49.451357008333318</v>
+      </c>
+      <c r="I9" s="15">
+        <f>DEVSQ(D9:D14)</f>
+        <v>471.45150430000012</v>
+      </c>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="59"/>
+      <c r="B10" s="46"/>
+      <c r="C10">
+        <v>16.75</v>
+      </c>
+      <c r="D10" s="7">
+        <v>22</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="32">
+        <f>DEVSQ(C15:C20)</f>
+        <v>42.088333333333331</v>
+      </c>
+      <c r="I10" s="15">
+        <f>DEVSQ(D15:D20)</f>
+        <v>59.188000000000009</v>
+      </c>
+      <c r="J10" s="35"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="46"/>
+      <c r="C11">
+        <v>20.5</v>
+      </c>
+      <c r="D11" s="7">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="59"/>
+      <c r="B12" s="46"/>
+      <c r="C12">
+        <v>26.597899999999999</v>
+      </c>
+      <c r="D12" s="7">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
+      <c r="B13" s="46"/>
+      <c r="C13">
+        <v>21.45</v>
+      </c>
+      <c r="D13" s="7">
+        <v>23.9</v>
+      </c>
+      <c r="G13" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="59"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="6">
+        <v>21.45</v>
+      </c>
+      <c r="D14" s="8">
+        <v>43.715400000000002</v>
+      </c>
+      <c r="G14" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="59"/>
+      <c r="B15" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>12.6</v>
+      </c>
+      <c r="D15" s="7">
+        <v>12.3</v>
+      </c>
+      <c r="G15" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
+      <c r="B16" s="46"/>
+      <c r="C16">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D16" s="7">
+        <v>18.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
+      <c r="B17" s="46"/>
+      <c r="C17">
+        <v>10.6</v>
+      </c>
+      <c r="D17" s="7">
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="59"/>
+      <c r="B18" s="46"/>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7">
+        <v>19</v>
+      </c>
+      <c r="F18" s="84" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="59"/>
+      <c r="B19" s="46"/>
+      <c r="C19">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D19" s="7">
+        <v>12.8</v>
+      </c>
+      <c r="F19" s="84"/>
+      <c r="G19" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="68">
+        <f>C24*DEVSQ(H2:I4)</f>
+        <v>1425.3359078222227</v>
+      </c>
+      <c r="I19" s="79">
+        <f>A24*B24-1</f>
+        <v>5</v>
+      </c>
+      <c r="J19" s="80">
+        <f>H19/I19</f>
+        <v>285.06718156444452</v>
+      </c>
+      <c r="K19" s="79">
+        <f>J19/J20</f>
+        <v>11.128931039835519</v>
+      </c>
+      <c r="L19" s="81">
+        <f>_xlfn.F.DIST.RT(K19,I19,I20)</f>
+        <v>3.9779163995544241E-6</v>
+      </c>
+      <c r="M19" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" s="8" t="str">
+        <f>IF(L19&lt;$E$24, "Rejected", "Cannot Reject")</f>
+        <v>Rejected</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="59"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="6">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D20" s="8">
+        <v>11.92</v>
+      </c>
+      <c r="F20" s="84"/>
+      <c r="G20" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="32">
+        <f>SUM(H8:I10)</f>
+        <v>768.44895671666688</v>
+      </c>
+      <c r="I20" s="39">
+        <f>D24-A24*B24</f>
+        <v>30</v>
+      </c>
+      <c r="J20" s="8">
+        <f>H20/I20</f>
+        <v>25.614965223888895</v>
+      </c>
+      <c r="K20" s="40"/>
+      <c r="L20" s="24"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G21" s="82"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="39">
+        <v>3</v>
+      </c>
+      <c r="B24" s="8">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8">
+        <v>6</v>
+      </c>
+      <c r="D24" s="8">
+        <f>COUNT(C3:D20)</f>
+        <v>36</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G24" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="30">
+        <f>H2-$J$5</f>
+        <v>8.9415499999999994</v>
+      </c>
+      <c r="I24" s="70">
+        <f>I2-$J$5</f>
+        <v>13.29</v>
+      </c>
+      <c r="J24" s="31">
+        <f>SUM(H24:I26)</f>
+        <v>93.320433333333327</v>
+      </c>
+      <c r="K24" s="31">
+        <f>J5</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="31">
+        <f>J20</f>
+        <v>25.614965223888895</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G25" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="32">
+        <f>H3-$J$5</f>
+        <v>21.366316666666666</v>
+      </c>
+      <c r="I25" s="71">
+        <f>I3-$J$5</f>
+        <v>26.235900000000004</v>
+      </c>
+      <c r="J25" s="73"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="77"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G26" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H26" s="33">
+        <f>H4-$J$5</f>
+        <v>9.3166666666666682</v>
+      </c>
+      <c r="I26" s="72">
+        <f>I4-$J$5</f>
+        <v>14.17</v>
+      </c>
+      <c r="J26" s="75"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="78"/>
+    </row>
+    <row r="29" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="M29" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" s="28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="84"/>
+      <c r="G30" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="68">
+        <f>C24*DEVSQ(H24:I26)</f>
+        <v>1425.3359078222227</v>
+      </c>
+      <c r="I30" s="79">
+        <f>A24*B24-1</f>
+        <v>5</v>
+      </c>
+      <c r="J30" s="80">
+        <f>H30/I30</f>
+        <v>285.06718156444452</v>
+      </c>
+      <c r="K30" s="79">
+        <f>J30/J31</f>
+        <v>11.128931039835519</v>
+      </c>
+      <c r="L30" s="79">
+        <f>_xlfn.F.DIST.RT(K30,I30,I31)</f>
+        <v>3.9779163995544241E-6</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="8" t="str">
+        <f>IF(L19&lt;$E$24, "Rejected", "Cannot Reject")</f>
+        <v>Rejected</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F31" s="84"/>
+      <c r="G31" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="86">
+        <f>SUM(H8:I10)</f>
+        <v>768.44895671666688</v>
+      </c>
+      <c r="I31" s="39">
+        <f>D24-A24*B24</f>
+        <v>30</v>
+      </c>
+      <c r="J31" s="8">
+        <f>H31/I31</f>
+        <v>25.614965223888895</v>
+      </c>
+      <c r="K31" s="40"/>
+      <c r="L31" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="J25:L26"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="B15:B20"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N30">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Rejected">
+      <formula>NOT(ISERROR(SEARCH("Rejected",N30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" stopIfTrue="1" operator="containsText" text="Cannot Reject">
+      <formula>NOT(ISERROR(SEARCH("Cannot Reject",N30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Rejected">
+      <formula>NOT(ISERROR(SEARCH("Rejected",N19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" stopIfTrue="1" operator="containsText" text="Cannot Reject">
+      <formula>NOT(ISERROR(SEARCH("Cannot Reject",N19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F43188-026E-7742-AA92-2FD306518DEB}">
+  <dimension ref="A1:N32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="44"/>
+      <c r="G1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="11">
+        <f>AVERAGE(C3:C8)</f>
+        <v>8.9415499999999994</v>
+      </c>
+      <c r="I2" s="11">
+        <f>AVERAGE(D3:D8)</f>
+        <v>13.29</v>
+      </c>
+      <c r="J2" s="12">
         <f>AVERAGE(C3:D8)</f>
         <v>11.115775000000001</v>
       </c>
-      <c r="K2" s="32">
+      <c r="K2" s="13">
         <f>J2-$J$5</f>
         <v>-4.437630555555554</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="46" t="s">
         <v>4</v>
       </c>
       <c r="C3">
         <v>5.25</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="7">
         <v>11.75</v>
       </c>
-      <c r="G3" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="34">
+      <c r="F3" s="7"/>
+      <c r="G3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="15">
         <f>AVERAGE(C9:C14)</f>
         <v>21.366316666666666</v>
       </c>
-      <c r="I3" s="34">
+      <c r="I3" s="15">
         <f>AVERAGE(D9:D14)</f>
         <v>26.235900000000004</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="16">
         <f>AVERAGE(C9:D14)</f>
         <v>23.801108333333332</v>
       </c>
-      <c r="K3" s="45">
-        <f t="shared" ref="K3:K4" si="0">J3-$J$5</f>
+      <c r="K3" s="26">
+        <f>J3-$J$5</f>
         <v>8.2477027777777767</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
-      <c r="B4" s="8"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="59"/>
+      <c r="B4" s="46"/>
       <c r="C4">
         <v>12.1</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="7">
         <v>14.99</v>
       </c>
-      <c r="G4" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="36">
+      <c r="F4" s="7"/>
+      <c r="G4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="17">
         <f>AVERAGE(C15:C20)</f>
         <v>9.3166666666666682</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="17">
         <f>AVERAGE(D15:D20)</f>
         <v>14.17</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="16">
         <f>AVERAGE(C15:D20)</f>
         <v>11.743333333333332</v>
       </c>
-      <c r="K4" s="44">
-        <f t="shared" si="0"/>
+      <c r="K4" s="25">
+        <f>J4-$J$5</f>
         <v>-3.8100722222222227</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="47"/>
-      <c r="B5" s="8"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="59"/>
+      <c r="B5" s="46"/>
       <c r="C5">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="7">
         <v>7.65</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="19">
         <f>AVERAGE(C3:C20)</f>
         <v>13.208177777777776</v>
       </c>
-      <c r="I5" s="39">
+      <c r="I5" s="20">
         <f>AVERAGE(D3:D20)</f>
         <v>17.898633333333336</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="21">
         <f>AVERAGE(C3:D20)</f>
         <v>15.553405555555555</v>
       </c>
-      <c r="K5" s="41"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
-      <c r="B6" s="8"/>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="59"/>
+      <c r="B6" s="46"/>
       <c r="C6">
         <v>5.5993000000000004</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="7">
         <v>13.75</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="23">
         <f>H5-$J$5</f>
         <v>-2.3452277777777795</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="23">
         <f>I5-$J$5</f>
         <v>2.3452277777777812</v>
       </c>
-      <c r="J6" s="41"/>
-      <c r="K6" s="43"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
-      <c r="B7" s="8"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="59"/>
+      <c r="B7" s="46"/>
       <c r="C7">
         <v>8.5</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="17">
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+    </row>
+    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="59"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="6">
         <v>14</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="8">
         <v>11.6</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="G8" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="58"/>
-    </row>
-    <row r="9" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
-      <c r="B9" s="8" t="s">
+      <c r="H8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="34"/>
+    </row>
+    <row r="9" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="59"/>
+      <c r="B9" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C9">
         <v>21.45</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="7">
         <v>14.7</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="51">
+      <c r="F9" s="7"/>
+      <c r="G9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="30">
         <f>DEVSQ(C3:C8)</f>
         <v>61.106762074999999</v>
       </c>
-      <c r="I9" s="52">
+      <c r="I9" s="31">
         <f>DEVSQ(D3:D8)</f>
         <v>85.163000000000011</v>
       </c>
-      <c r="J9" s="59"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
-      <c r="B10" s="8"/>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="59"/>
+      <c r="B10" s="46"/>
       <c r="C10">
         <v>16.75</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="7">
         <v>22</v>
       </c>
-      <c r="G10" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="53">
+      <c r="F10" s="7"/>
+      <c r="G10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="32">
         <f>DEVSQ(C9:C14)</f>
         <v>49.451357008333318</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="15">
         <f>DEVSQ(D9:D14)</f>
         <v>471.45150430000012</v>
       </c>
-      <c r="J10" s="59"/>
-    </row>
-    <row r="11" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="8"/>
+      <c r="J10" s="35"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="46"/>
       <c r="C11">
         <v>20.5</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="7">
         <v>28.7</v>
       </c>
-      <c r="G11" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="53">
+      <c r="F11" s="7"/>
+      <c r="G11" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="32">
         <f>DEVSQ(C15:C20)</f>
         <v>42.088333333333331</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="15">
         <f>DEVSQ(D15:D20)</f>
         <v>59.188000000000009</v>
       </c>
-      <c r="J11" s="59"/>
-    </row>
-    <row r="12" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
-      <c r="B12" s="8"/>
+      <c r="J11" s="35"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="59"/>
+      <c r="B12" s="46"/>
       <c r="C12">
         <v>26.597899999999999</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="7">
         <v>24.4</v>
       </c>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="47"/>
-      <c r="B13" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="59"/>
+      <c r="B13" s="46"/>
       <c r="C13">
         <v>21.45</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="7">
         <v>23.9</v>
       </c>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="17">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="59"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="6">
         <v>21.45</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="8">
         <v>43.715400000000002</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="58"/>
-    </row>
-    <row r="15" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="47"/>
-      <c r="B15" s="8" t="s">
+      <c r="H14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="34"/>
+    </row>
+    <row r="15" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="59"/>
+      <c r="B15" s="46" t="s">
         <v>6</v>
       </c>
       <c r="C15">
         <v>12.6</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="7">
         <v>12.3</v>
       </c>
-      <c r="G15" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="51">
+      <c r="G15" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="30">
         <f>H2-$J2-H$5+$J$5</f>
         <v>0.17100277777777784</v>
       </c>
-      <c r="I15" s="52">
+      <c r="I15" s="31">
         <f>I2-$J2-I$5+$J$5</f>
         <v>-0.17100277777778317</v>
       </c>
-      <c r="J15" s="59"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="47"/>
-      <c r="B16" s="8"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
+      <c r="B16" s="46"/>
       <c r="C16">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="7">
         <v>18.05</v>
       </c>
-      <c r="G16" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="53">
-        <f t="shared" ref="H16:I16" si="1">H3-$J3-H$5+$J$5</f>
+      <c r="G16" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="32">
+        <f>H3-$J3-H$5+$J$5</f>
         <v>-8.9563888888886112E-2</v>
       </c>
-      <c r="I16" s="34">
-        <f t="shared" si="1"/>
+      <c r="I16" s="15">
+        <f>I3-$J3-I$5+$J$5</f>
         <v>8.9563888888891441E-2</v>
       </c>
-      <c r="J16" s="59"/>
-    </row>
-    <row r="17" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="8"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
+      <c r="B17" s="46"/>
       <c r="C17">
         <v>10.6</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="7">
         <v>10.95</v>
       </c>
-      <c r="G17" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="55">
-        <f t="shared" ref="H17:I17" si="2">H4-$J4-H$5+$J$5</f>
+      <c r="G17" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="33">
+        <f>H4-$J4-H$5+$J$5</f>
         <v>-8.143888888888462E-2</v>
       </c>
-      <c r="I17" s="36">
-        <f t="shared" si="2"/>
+      <c r="I17" s="17">
+        <f>I4-$J4-I$5+$J$5</f>
         <v>8.1438888888886396E-2</v>
       </c>
-      <c r="J17" s="59"/>
-    </row>
-    <row r="18" spans="1:15" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
-      <c r="B18" s="8"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="59"/>
+      <c r="B18" s="46"/>
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="7">
         <v>19</v>
       </c>
-      <c r="J18" s="16"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="47"/>
-      <c r="B19" s="8"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="59"/>
+      <c r="B19" s="46"/>
       <c r="C19">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="7">
         <v>12.8</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="57"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="47"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="17">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="59"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="6">
         <v>10.199999999999999</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="8">
         <v>11.92</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46" t="s">
+      <c r="K20" s="41"/>
+    </row>
+    <row r="23" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="60" t="s">
+      <c r="E23" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H23" s="49" t="s">
+      <c r="H23" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="50" t="s">
+      <c r="I23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="49" t="s">
+      <c r="K23" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="49" t="s">
+      <c r="L23" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="N23" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="O23" s="49" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="M23" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N23" s="28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="39">
         <v>3</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="8">
         <v>2</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="8">
         <v>6</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="8">
         <f>COUNT(C3:D20)</f>
         <v>36</v>
       </c>
-      <c r="G24" s="61" t="s">
+      <c r="E24" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G24" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H24" s="62">
-        <f>DEVSQ((K2:K4))*A24*C24</f>
-        <v>1840.2086951408326</v>
-      </c>
-      <c r="I24" s="63">
+      <c r="H24" s="38">
+        <f>DEVSQ((K2:K4))*B24*C24</f>
+        <v>1226.805796760555</v>
+      </c>
+      <c r="I24" s="39">
         <f>A24-1</f>
         <v>2</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="8">
         <f>H24/I24</f>
-        <v>920.10434757041628</v>
-      </c>
-      <c r="K24" s="19">
+        <v>613.40289838027752</v>
+      </c>
+      <c r="K24" s="8">
         <f>J24/$J$27</f>
-        <v>35.920577659512624</v>
-      </c>
-      <c r="L24" s="19">
+        <v>23.947051773008418</v>
+      </c>
+      <c r="L24" s="8">
         <f>_xlfn.F.DIST.RT(K24,I24,$I$27)</f>
-        <v>1.0913625804183809E-8</v>
-      </c>
-      <c r="N24">
-        <f>C24*DEVSQ(H2:I4)</f>
-        <v>1425.3359078222227</v>
-      </c>
-      <c r="O24">
-        <f>SUM(H24:H26)</f>
-        <v>1972.7376862465737</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G25" s="61" t="s">
+        <v>6.0848526739443857E-7</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N24" s="8" t="str">
+        <f>IF(L24&lt;$E$24, "Rejected", "Cannot Reject")</f>
+        <v>Rejected</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G25" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="62">
-        <f>DEVSQ(H6:I6)*B24*C24</f>
-        <v>132.00223991185214</v>
-      </c>
-      <c r="I25" s="63">
+      <c r="H25" s="38">
+        <f>DEVSQ(H6:I6)*A24*C24</f>
+        <v>198.00335986777822</v>
+      </c>
+      <c r="I25" s="39">
         <f>B24-1</f>
         <v>1</v>
       </c>
-      <c r="J25" s="19">
-        <f t="shared" ref="J25:J27" si="3">H25/I25</f>
-        <v>132.00223991185214</v>
-      </c>
-      <c r="K25" s="19">
-        <f t="shared" ref="K25:K26" si="4">J25/$J$27</f>
-        <v>5.1533249706989608</v>
-      </c>
-      <c r="L25" s="19">
-        <f t="shared" ref="L25:L26" si="5">_xlfn.F.DIST.RT(K25,I25,$I$27)</f>
-        <v>3.0549321697915566E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G26" s="61" t="s">
+      <c r="J25" s="8">
+        <f>H25/I25</f>
+        <v>198.00335986777822</v>
+      </c>
+      <c r="K25" s="8">
+        <f>J25/$J$27</f>
+        <v>7.7299874560484412</v>
+      </c>
+      <c r="L25" s="8">
+        <f>_xlfn.F.DIST.RT(K25,I25,$I$27)</f>
+        <v>9.2897133503825075E-3</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N25" s="8" t="str">
+        <f>IF(L25&lt;$E$24, "Rejected", "Cannot Reject")</f>
+        <v>Rejected</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G26" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="62">
+      <c r="H26" s="38">
         <f>DEVSQ(H15:I17)*C24</f>
         <v>0.52675119388889324</v>
       </c>
-      <c r="I26" s="63">
+      <c r="I26" s="39">
         <f>I24*I25</f>
         <v>2</v>
       </c>
-      <c r="J26" s="19">
-        <f t="shared" si="3"/>
+      <c r="J26" s="8">
+        <f>H26/I26</f>
         <v>0.26337559694444662</v>
       </c>
-      <c r="K26" s="19">
-        <f t="shared" si="4"/>
+      <c r="K26" s="8">
+        <f>J26/$J$27</f>
         <v>1.0282098556152582E-2</v>
       </c>
-      <c r="L26" s="19">
-        <f t="shared" si="5"/>
+      <c r="L26" s="8">
+        <f>_xlfn.F.DIST.RT(K26,I26,$I$27)</f>
         <v>0.98977406792642231</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G27" s="61" t="s">
+      <c r="M26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" s="8" t="str">
+        <f>IF(L26&lt;$E$24, "Rejected", "Cannot Reject")</f>
+        <v>Cannot Reject</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G27" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="H27" s="53">
+      <c r="H27" s="86">
         <f>SUM(H9:I11)</f>
         <v>768.44895671666688</v>
       </c>
-      <c r="I27" s="63">
-        <f>D24-A24*B24</f>
+      <c r="I27" s="39">
+        <f>D24-(A24*B24)</f>
         <v>30</v>
       </c>
-      <c r="J27" s="19">
-        <f t="shared" si="3"/>
+      <c r="J27" s="8">
+        <f>H27/I27</f>
         <v>25.614965223888895</v>
       </c>
-      <c r="K27" s="64"/>
-      <c r="L27" s="43"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="24"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G28" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="38">
+        <f>DEVSQ(C3:D20)</f>
+        <v>2193.784864538889</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G29" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="38">
+        <f>SUM(H24:H27)</f>
+        <v>2193.784864538889</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" s="56"/>
+    </row>
+    <row r="32" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="G32" s="39">
+        <f>C24*(DEVSQ(H2:I4))</f>
+        <v>1425.3359078222227</v>
+      </c>
+      <c r="H32" s="57">
+        <f>SUM(H24:H26)</f>
+        <v>1425.3359078222222</v>
+      </c>
+      <c r="I32" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A3:A20"/>
     <mergeCell ref="B3:B8"/>
@@ -4471,7 +5768,16 @@
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="A1:B2"/>
   </mergeCells>
+  <conditionalFormatting sqref="N24:N26">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Rejected">
+      <formula>NOT(ISERROR(SEARCH("Rejected",N24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="8" stopIfTrue="1" operator="containsText" text="Cannot Reject">
+      <formula>NOT(ISERROR(SEARCH("Cannot Reject",N24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>